<commit_message>
[DHTD-76] Risk Management Table Sorting Update
</commit_message>
<xml_diff>
--- a/documents/RiskManagement.xlsx
+++ b/documents/RiskManagement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programmierung\Android\Tower-Defense\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDB9640-4317-4305-9FC7-68966055FACF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC00F59C-5908-44A5-A266-6E10FBA938C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-165" yWindow="-165" windowWidth="29130" windowHeight="15930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -251,9 +251,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -270,6 +267,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -562,7 +562,7 @@
   <cols>
     <col min="1" max="1" width="4.08984375" customWidth="1"/>
     <col min="2" max="2" width="20.54296875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.90625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="39.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="15.90625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.90625" style="1" bestFit="1" customWidth="1"/>
@@ -574,61 +574,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="29" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
       <c r="M1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" s="6">
+    <row r="2" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1</v>
-      </c>
-      <c r="E2" s="7">
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6">
         <v>3</v>
       </c>
       <c r="F2" s="8">
         <f>D2*E2</f>
-        <v>3</v>
-      </c>
-      <c r="G2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" s="6" t="s">
         <v>37</v>
       </c>
       <c r="J2" t="s">
@@ -641,192 +641,192 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="7">
-        <v>1</v>
-      </c>
-      <c r="E3" s="7">
-        <v>3</v>
-      </c>
-      <c r="F3" s="8">
+      <c r="B3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2</v>
+      </c>
+      <c r="E3" s="6">
+        <v>2</v>
+      </c>
+      <c r="F3" s="7">
         <f>D3*E3</f>
-        <v>3</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="6">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="7">
-        <v>2</v>
-      </c>
-      <c r="E4" s="7">
-        <v>2</v>
-      </c>
-      <c r="F4" s="8">
+      <c r="B4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="7">
         <f>D4*E4</f>
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="G4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>38</v>
+      <c r="B5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="6">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <f>D5*E5</f>
+        <v>3</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="7">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="6">
         <v>3</v>
       </c>
-      <c r="F5" s="9">
-        <f t="shared" ref="F5:F9" si="0">D5*E5</f>
+      <c r="F6" s="7">
+        <f>D6*E6</f>
+        <v>3</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="7">
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
-        <v>3</v>
-      </c>
-      <c r="F6" s="8">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="7">
-        <v>2</v>
-      </c>
-      <c r="F7" s="10">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="E7" s="6">
+        <v>2</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" ref="F5:F9" si="0">D7*E7</f>
+        <v>2</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="6">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="7">
-        <v>2</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="D8" s="6">
+        <v>2</v>
+      </c>
+      <c r="E8" s="6">
         <v>1</v>
       </c>
-      <c r="F8" s="10">
+      <c r="F8" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="6">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>1</v>
       </c>
-      <c r="E9" s="7">
-        <v>2</v>
-      </c>
-      <c r="F9" s="10">
+      <c r="E9" s="6">
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="6" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>